<commit_message>
Updated degradation curves: all chemistries equal
</commit_message>
<xml_diff>
--- a/data/raw_data/degradation_curves_slb.xlsx
+++ b/data/raw_data/degradation_curves_slb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61FC8ED-A707-104E-AB11-D1CCEDDE8C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD65BB-78DC-D544-8809-5FF9B46F6A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
   </bookViews>
@@ -527,97 +527,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0.84999999999999987</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78999999999999992</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7599999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.73</c:v>
+                  <c:v>0.64000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66999999999999993</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6399999999999999</c:v>
+                  <c:v>0.52000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61</c:v>
+                  <c:v>0.48000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.44000000000000017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.40000000000000019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.52</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.43</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.4</c:v>
+                  <c:v>0.19999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.37000000000000099</c:v>
+                  <c:v>0.159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.34000000000000102</c:v>
+                  <c:v>0.119999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.310000000000002</c:v>
+                  <c:v>7.99999999999991E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.28000000000000203</c:v>
+                  <c:v>3.9999999999999002E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.250000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.220000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.190000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.160000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.130000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.100000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.0000000000001797E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0000000000001798E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,97 +1264,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0.84999999999999987</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78999999999999992</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7599999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.73</c:v>
+                  <c:v>0.64000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66999999999999993</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6399999999999999</c:v>
+                  <c:v>0.52000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61</c:v>
+                  <c:v>0.48000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.44000000000000017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.40000000000000019</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.52</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.43</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.4</c:v>
+                  <c:v>0.19999999999999901</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.37000000000000099</c:v>
+                  <c:v>0.159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.34000000000000102</c:v>
+                  <c:v>0.119999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.310000000000002</c:v>
+                  <c:v>7.99999999999991E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.28000000000000203</c:v>
+                  <c:v>3.9999999999999002E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.250000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.220000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.190000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.160000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.130000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.100000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.0000000000001797E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0000000000001798E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.00000000000019E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3176,7 +3176,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3203,7 +3203,7 @@
         <v>0.8</v>
       </c>
       <c r="C2">
-        <v>0.84999999999999987</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3214,7 +3214,7 @@
         <v>0.76</v>
       </c>
       <c r="C3">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
         <v>0.72</v>
       </c>
       <c r="C4">
-        <v>0.78999999999999992</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3236,7 +3236,7 @@
         <v>0.68</v>
       </c>
       <c r="C5">
-        <v>0.7599999999999999</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3247,7 +3247,7 @@
         <v>0.64000000000000012</v>
       </c>
       <c r="C6">
-        <v>0.73</v>
+        <v>0.64000000000000012</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3258,7 +3258,7 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="C7">
-        <v>0.7</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3269,7 +3269,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C8">
-        <v>0.66999999999999993</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3280,7 +3280,7 @@
         <v>0.52000000000000013</v>
       </c>
       <c r="C9">
-        <v>0.6399999999999999</v>
+        <v>0.52000000000000013</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3291,7 +3291,7 @@
         <v>0.48000000000000015</v>
       </c>
       <c r="C10">
-        <v>0.61</v>
+        <v>0.48000000000000015</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3302,7 +3302,7 @@
         <v>0.44000000000000017</v>
       </c>
       <c r="C11">
-        <v>0.57999999999999996</v>
+        <v>0.44000000000000017</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3313,7 +3313,7 @@
         <v>0.40000000000000019</v>
       </c>
       <c r="C12">
-        <v>0.55000000000000004</v>
+        <v>0.40000000000000019</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3324,7 +3324,7 @@
         <v>0.36</v>
       </c>
       <c r="C13">
-        <v>0.52</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3335,7 +3335,7 @@
         <v>0.32</v>
       </c>
       <c r="C14">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3346,7 +3346,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="C15">
-        <v>0.46</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3357,7 +3357,7 @@
         <v>0.24</v>
       </c>
       <c r="C16">
-        <v>0.43</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3368,7 +3368,7 @@
         <v>0.19999999999999901</v>
       </c>
       <c r="C17">
-        <v>0.4</v>
+        <v>0.19999999999999901</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3379,7 +3379,7 @@
         <v>0.159999999999999</v>
       </c>
       <c r="C18">
-        <v>0.37000000000000099</v>
+        <v>0.159999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>0.119999999999999</v>
       </c>
       <c r="C19">
-        <v>0.34000000000000102</v>
+        <v>0.119999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3401,7 +3401,7 @@
         <v>7.99999999999991E-2</v>
       </c>
       <c r="C20">
-        <v>0.310000000000002</v>
+        <v>7.99999999999991E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3412,7 +3412,7 @@
         <v>3.9999999999999002E-2</v>
       </c>
       <c r="C21">
-        <v>0.28000000000000203</v>
+        <v>3.9999999999999002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3423,7 +3423,7 @@
         <v>0.01</v>
       </c>
       <c r="C22">
-        <v>0.250000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3434,7 +3434,7 @@
         <v>0.01</v>
       </c>
       <c r="C23">
-        <v>0.220000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3445,7 +3445,7 @@
         <v>0.01</v>
       </c>
       <c r="C24">
-        <v>0.190000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3456,7 +3456,7 @@
         <v>0.01</v>
       </c>
       <c r="C25">
-        <v>0.160000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3467,7 +3467,7 @@
         <v>0.01</v>
       </c>
       <c r="C26">
-        <v>0.130000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3478,7 +3478,7 @@
         <v>0.01</v>
       </c>
       <c r="C27">
-        <v>0.100000000000002</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3489,7 +3489,7 @@
         <v>0.01</v>
       </c>
       <c r="C28">
-        <v>7.0000000000001797E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3500,7 +3500,7 @@
         <v>0.01</v>
       </c>
       <c r="C29">
-        <v>4.0000000000001798E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3511,7 +3511,7 @@
         <v>0.01</v>
       </c>
       <c r="C30">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3522,7 +3522,7 @@
         <v>0.01</v>
       </c>
       <c r="C31">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3533,7 +3533,7 @@
         <v>0.01</v>
       </c>
       <c r="C32">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3544,7 +3544,7 @@
         <v>0.01</v>
       </c>
       <c r="C33">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3555,7 +3555,7 @@
         <v>0.01</v>
       </c>
       <c r="C34">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,7 +3566,7 @@
         <v>0.01</v>
       </c>
       <c r="C35">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3577,7 +3577,7 @@
         <v>0.01</v>
       </c>
       <c r="C36">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3588,7 +3588,7 @@
         <v>0.01</v>
       </c>
       <c r="C37">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3599,7 +3599,7 @@
         <v>0.01</v>
       </c>
       <c r="C38">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3610,7 +3610,7 @@
         <v>0.01</v>
       </c>
       <c r="C39">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3621,7 +3621,7 @@
         <v>0.01</v>
       </c>
       <c r="C40">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
         <v>0.01</v>
       </c>
       <c r="C41">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3643,7 +3643,7 @@
         <v>0.01</v>
       </c>
       <c r="C42">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3654,7 +3654,7 @@
         <v>0.01</v>
       </c>
       <c r="C43">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3665,7 +3665,7 @@
         <v>0.01</v>
       </c>
       <c r="C44">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3676,7 +3676,7 @@
         <v>0.01</v>
       </c>
       <c r="C45">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -3687,7 +3687,7 @@
         <v>0.01</v>
       </c>
       <c r="C46">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3698,7 +3698,7 @@
         <v>0.01</v>
       </c>
       <c r="C47">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3709,7 +3709,7 @@
         <v>0.01</v>
       </c>
       <c r="C48">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3720,7 +3720,7 @@
         <v>0.01</v>
       </c>
       <c r="C49">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3731,7 +3731,7 @@
         <v>0.01</v>
       </c>
       <c r="C50">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3742,7 +3742,7 @@
         <v>0.01</v>
       </c>
       <c r="C51">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3753,7 +3753,7 @@
         <v>0.01</v>
       </c>
       <c r="C52">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3764,7 +3764,7 @@
         <v>0.01</v>
       </c>
       <c r="C53">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3775,7 +3775,7 @@
         <v>0.01</v>
       </c>
       <c r="C54">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3786,7 +3786,7 @@
         <v>0.01</v>
       </c>
       <c r="C55">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3797,7 +3797,7 @@
         <v>0.01</v>
       </c>
       <c r="C56">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3808,7 +3808,7 @@
         <v>0.01</v>
       </c>
       <c r="C57">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3819,7 +3819,7 @@
         <v>0.01</v>
       </c>
       <c r="C58">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3830,7 +3830,7 @@
         <v>0.01</v>
       </c>
       <c r="C59">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3841,7 +3841,7 @@
         <v>0.01</v>
       </c>
       <c r="C60">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3852,7 +3852,7 @@
         <v>0.01</v>
       </c>
       <c r="C61">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3863,7 +3863,7 @@
         <v>0.01</v>
       </c>
       <c r="C62">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3874,7 +3874,7 @@
         <v>0.01</v>
       </c>
       <c r="C63">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -3885,7 +3885,7 @@
         <v>0.01</v>
       </c>
       <c r="C64">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -3896,7 +3896,7 @@
         <v>0.01</v>
       </c>
       <c r="C65">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -3907,7 +3907,7 @@
         <v>0.01</v>
       </c>
       <c r="C66">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -3918,7 +3918,7 @@
         <v>0.01</v>
       </c>
       <c r="C67">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -3929,7 +3929,7 @@
         <v>0.01</v>
       </c>
       <c r="C68">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -3940,7 +3940,7 @@
         <v>0.01</v>
       </c>
       <c r="C69">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -3951,7 +3951,7 @@
         <v>0.01</v>
       </c>
       <c r="C70">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -3962,7 +3962,7 @@
         <v>0.01</v>
       </c>
       <c r="C71">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -3973,7 +3973,7 @@
         <v>0.01</v>
       </c>
       <c r="C72">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -3984,7 +3984,7 @@
         <v>0.01</v>
       </c>
       <c r="C73">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -3995,7 +3995,7 @@
         <v>0.01</v>
       </c>
       <c r="C74">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -4006,7 +4006,7 @@
         <v>0.01</v>
       </c>
       <c r="C75">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -4017,7 +4017,7 @@
         <v>0.01</v>
       </c>
       <c r="C76">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -4028,7 +4028,7 @@
         <v>0.01</v>
       </c>
       <c r="C77">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -4039,7 +4039,7 @@
         <v>0.01</v>
       </c>
       <c r="C78">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -4050,7 +4050,7 @@
         <v>0.01</v>
       </c>
       <c r="C79">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -4061,7 +4061,7 @@
         <v>0.01</v>
       </c>
       <c r="C80">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -4072,7 +4072,7 @@
         <v>0.01</v>
       </c>
       <c r="C81">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -4083,7 +4083,7 @@
         <v>0.01</v>
       </c>
       <c r="C82">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -4094,7 +4094,7 @@
         <v>0.01</v>
       </c>
       <c r="C83">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -4105,7 +4105,7 @@
         <v>0.01</v>
       </c>
       <c r="C84">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -4116,7 +4116,7 @@
         <v>0.01</v>
       </c>
       <c r="C85">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -4127,7 +4127,7 @@
         <v>0.01</v>
       </c>
       <c r="C86">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4138,7 +4138,7 @@
         <v>0.01</v>
       </c>
       <c r="C87">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -4149,7 +4149,7 @@
         <v>0.01</v>
       </c>
       <c r="C88">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -4160,7 +4160,7 @@
         <v>0.01</v>
       </c>
       <c r="C89">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -4171,7 +4171,7 @@
         <v>0.01</v>
       </c>
       <c r="C90">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -4182,7 +4182,7 @@
         <v>0.01</v>
       </c>
       <c r="C91">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,7 +4193,7 @@
         <v>0.01</v>
       </c>
       <c r="C92">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4204,7 +4204,7 @@
         <v>0.01</v>
       </c>
       <c r="C93">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -4215,7 +4215,7 @@
         <v>0.01</v>
       </c>
       <c r="C94">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -4226,7 +4226,7 @@
         <v>0.01</v>
       </c>
       <c r="C95">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -4237,7 +4237,7 @@
         <v>0.01</v>
       </c>
       <c r="C96">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>0.01</v>
       </c>
       <c r="C97">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -4259,7 +4259,7 @@
         <v>0.01</v>
       </c>
       <c r="C98">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -4270,7 +4270,7 @@
         <v>0.01</v>
       </c>
       <c r="C99">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -4281,7 +4281,7 @@
         <v>0.01</v>
       </c>
       <c r="C100">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -4292,7 +4292,7 @@
         <v>0.01</v>
       </c>
       <c r="C101">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -4303,7 +4303,7 @@
         <v>0.01</v>
       </c>
       <c r="C102">
-        <v>1.00000000000019E-2</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>